<commit_message>
Gmail validation was done
</commit_message>
<xml_diff>
--- a/workspace/Appium_Android/testCaseExcel/gmailUserCredential.xlsx
+++ b/workspace/Appium_Android/testCaseExcel/gmailUserCredential.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>jakay00734@gmail.com</t>
   </si>
   <si>
@@ -40,6 +37,30 @@
   </si>
   <si>
     <t>jakay507@gmail.com</t>
+  </si>
+  <si>
+    <t>Actual_Result</t>
+  </si>
+  <si>
+    <t>Expected_Result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Sorry, Google doesn't recognize that email.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrong password. Try again. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter your password. </t>
+  </si>
+  <si>
+    <t>Please enter your email.</t>
+  </si>
+  <si>
+    <t>Please enter a valid email address.</t>
   </si>
 </sst>
 </file>
@@ -62,12 +83,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,10 +113,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,50 +413,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C2" sqref="C2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -436,12 +478,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>